<commit_message>
Adding mine and varuns changes
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/reports/Attendance_U08EMGH3ZUK_from_Mar-2023_to_Mar-2025.xlsx
+++ b/backend/slack-hrbp/reports/Attendance_U08EMGH3ZUK_from_Mar-2023_to_Mar-2025.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="842">
   <si>
     <t>Mar-2023 (Leave Date)</t>
   </si>
@@ -1676,6 +1676,9 @@
     <t>2025-03-20</t>
   </si>
   <si>
+    <t>Unplanned Leave</t>
+  </si>
+  <si>
     <t>2023-03-21</t>
   </si>
   <si>
@@ -2460,6 +2463,81 @@
   </si>
   <si>
     <t>2025-03-31</t>
+  </si>
+  <si>
+    <t>Mar-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Apr-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>May-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Jun-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Jul-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Aug-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Sep-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Oct-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Nov-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Dec-2023 Leave Summary</t>
+  </si>
+  <si>
+    <t>Jan-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Feb-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Mar-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Apr-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>May-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Jun-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Jul-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Aug-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Sep-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Oct-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Nov-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Dec-2024 Leave Summary</t>
+  </si>
+  <si>
+    <t>Jan-2025 Leave Summary</t>
+  </si>
+  <si>
+    <t>Feb-2025 Leave Summary</t>
+  </si>
+  <si>
+    <t>Mar-2025 Leave Summary</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AX32"/>
+  <dimension ref="A1:AX39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2558,7 +2636,7 @@
     <col min="46" max="46" width="20.890625" customWidth="true" bestFit="true"/>
     <col min="47" max="47" width="21.16015625" customWidth="true" bestFit="true"/>
     <col min="48" max="48" width="21.2421875" customWidth="true" bestFit="true"/>
-    <col min="49" max="49" width="21.6015625" customWidth="true" bestFit="true"/>
+    <col min="49" max="49" width="24.52734375" customWidth="true" bestFit="true"/>
     <col min="50" max="50" width="21.68359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -5751,460 +5829,460 @@
         <v>553</v>
       </c>
       <c r="AX21" t="s" s="0">
-        <v>51</v>
+        <v>554</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="H22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="J22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K22" t="s" s="0">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="L22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M22" t="s" s="0">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O22" t="s" s="0">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="P22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q22" t="s" s="0">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="R22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S22" t="s" s="0">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="T22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U22" t="s" s="0">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="V22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W22" t="s" s="0">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="X22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y22" t="s" s="0">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="Z22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA22" t="s" s="0">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="AB22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC22" t="s" s="0">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="AD22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE22" t="s" s="0">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="AF22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG22" t="s" s="0">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="AH22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI22" t="s" s="0">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="AJ22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK22" t="s" s="0">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AL22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM22" t="s" s="0">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AN22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO22" t="s" s="0">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="AP22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ22" t="s" s="0">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="AR22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS22" t="s" s="0">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="AT22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU22" t="s" s="0">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="AV22" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW22" t="s" s="0">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="AX22" t="s" s="0">
-        <v>51</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="H23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="J23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K23" t="s" s="0">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="L23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M23" t="s" s="0">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="N23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O23" t="s" s="0">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q23" t="s" s="0">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="R23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S23" t="s" s="0">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="T23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U23" t="s" s="0">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="V23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W23" t="s" s="0">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="X23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y23" t="s" s="0">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="Z23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA23" t="s" s="0">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="AB23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC23" t="s" s="0">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="AD23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE23" t="s" s="0">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="AF23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG23" t="s" s="0">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AH23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI23" t="s" s="0">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="AJ23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK23" t="s" s="0">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="AL23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM23" t="s" s="0">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="AN23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO23" t="s" s="0">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="AP23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ23" t="s" s="0">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="AR23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS23" t="s" s="0">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="AT23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU23" t="s" s="0">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="AV23" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW23" t="s" s="0">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="AX23" t="s" s="0">
-        <v>51</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="J24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K24" t="s" s="0">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="L24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M24" t="s" s="0">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="N24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O24" t="s" s="0">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="P24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q24" t="s" s="0">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="R24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S24" t="s" s="0">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="T24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U24" t="s" s="0">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="V24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W24" t="s" s="0">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="X24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y24" t="s" s="0">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="Z24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA24" t="s" s="0">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="AB24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC24" t="s" s="0">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="AD24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE24" t="s" s="0">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="AF24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG24" t="s" s="0">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="AH24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI24" t="s" s="0">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="AJ24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK24" t="s" s="0">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="AL24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM24" t="s" s="0">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AN24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO24" t="s" s="0">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="AP24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ24" t="s" s="0">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="AR24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS24" t="s" s="0">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="AT24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU24" t="s" s="0">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="AV24" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW24" t="s" s="0">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="AX24" t="s" s="0">
         <v>51</v>
@@ -6212,607 +6290,607 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="J25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K25" t="s" s="0">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="L25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M25" t="s" s="0">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="N25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O25" t="s" s="0">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q25" t="s" s="0">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="R25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S25" t="s" s="0">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="T25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U25" t="s" s="0">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="V25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W25" t="s" s="0">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="X25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y25" t="s" s="0">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="Z25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA25" t="s" s="0">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="AB25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC25" t="s" s="0">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="AD25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE25" t="s" s="0">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="AF25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG25" t="s" s="0">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="AH25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI25" t="s" s="0">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="AJ25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK25" t="s" s="0">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="AL25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM25" t="s" s="0">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="AN25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO25" t="s" s="0">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="AP25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ25" t="s" s="0">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="AR25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS25" t="s" s="0">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="AT25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU25" t="s" s="0">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="AV25" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW25" t="s" s="0">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="AX25" t="s" s="0">
-        <v>302</v>
+        <v>554</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="J26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K26" t="s" s="0">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M26" t="s" s="0">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="N26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O26" t="s" s="0">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="P26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q26" t="s" s="0">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="R26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S26" t="s" s="0">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="T26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U26" t="s" s="0">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="V26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W26" t="s" s="0">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="X26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y26" t="s" s="0">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="Z26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA26" t="s" s="0">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="AB26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC26" t="s" s="0">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="AD26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE26" t="s" s="0">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="AF26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG26" t="s" s="0">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="AH26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI26" t="s" s="0">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="AJ26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK26" t="s" s="0">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="AL26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM26" t="s" s="0">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="AN26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO26" t="s" s="0">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="AP26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ26" t="s" s="0">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="AR26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS26" t="s" s="0">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="AT26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU26" t="s" s="0">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AV26" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW26" t="s" s="0">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AX26" t="s" s="0">
-        <v>302</v>
+        <v>554</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="F27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="J27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K27" t="s" s="0">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="L27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M27" t="s" s="0">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="N27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O27" t="s" s="0">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q27" t="s" s="0">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="R27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S27" t="s" s="0">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="T27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U27" t="s" s="0">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="V27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W27" t="s" s="0">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="X27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y27" t="s" s="0">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="Z27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA27" t="s" s="0">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="AB27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC27" t="s" s="0">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="AD27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE27" t="s" s="0">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="AF27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG27" t="s" s="0">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="AH27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI27" t="s" s="0">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="AJ27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK27" t="s" s="0">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="AL27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM27" t="s" s="0">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="AN27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO27" t="s" s="0">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="AP27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ27" t="s" s="0">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="AR27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS27" t="s" s="0">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="AT27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU27" t="s" s="0">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="AV27" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW27" t="s" s="0">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="AX27" t="s" s="0">
-        <v>51</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="F28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G28" t="s" s="0">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="J28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K28" t="s" s="0">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="L28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="N28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O28" t="s" s="0">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="P28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q28" t="s" s="0">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="R28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S28" t="s" s="0">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="T28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U28" t="s" s="0">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="V28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W28" t="s" s="0">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="X28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y28" t="s" s="0">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="Z28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA28" t="s" s="0">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="AB28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC28" t="s" s="0">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="AD28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE28" t="s" s="0">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="AF28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG28" t="s" s="0">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="AH28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI28" t="s" s="0">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="AJ28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK28" t="s" s="0">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="AL28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM28" t="s" s="0">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="AN28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO28" t="s" s="0">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="AP28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ28" t="s" s="0">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="AR28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS28" t="s" s="0">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="AT28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU28" t="s" s="0">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="AV28" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW28" t="s" s="0">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="AX28" t="s" s="0">
         <v>51</v>
@@ -6820,151 +6898,151 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G29" t="s" s="0">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="J29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K29" t="s" s="0">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="L29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M29" t="s" s="0">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="N29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O29" t="s" s="0">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="P29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q29" t="s" s="0">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="R29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S29" t="s" s="0">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="T29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U29" t="s" s="0">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="V29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W29" t="s" s="0">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="X29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y29" t="s" s="0">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="Z29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA29" t="s" s="0">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="AB29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC29" t="s" s="0">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="AD29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE29" t="s" s="0">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="AF29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG29" t="s" s="0">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="AH29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI29" t="s" s="0">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="AJ29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK29" t="s" s="0">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="AL29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM29" t="s" s="0">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="AN29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO29" t="s" s="0">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="AP29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ29" t="s" s="0">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="AR29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS29" t="s" s="0">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="AT29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AU29" t="s" s="0">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="AV29" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW29" t="s" s="0">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="AX29" t="s" s="0">
         <v>51</v>
@@ -6972,145 +7050,145 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G30" t="s" s="0">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="H30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="J30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K30" t="s" s="0">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="L30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M30" t="s" s="0">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="N30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O30" t="s" s="0">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="P30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q30" t="s" s="0">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="R30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S30" t="s" s="0">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="T30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U30" t="s" s="0">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="V30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="W30" t="s" s="0">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="X30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y30" t="s" s="0">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="Z30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA30" t="s" s="0">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="AB30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC30" t="s" s="0">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AD30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE30" t="s" s="0">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AF30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG30" t="s" s="0">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AH30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI30" t="s" s="0">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AJ30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK30" t="s" s="0">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AL30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM30" t="s" s="0">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="AN30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO30" t="s" s="0">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="AP30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ30" t="s" s="0">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="AR30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS30" t="s" s="0">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="AT30" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW30" t="s" s="0">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="AX30" t="s" s="0">
         <v>51</v>
@@ -7118,139 +7196,139 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="F31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="H31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="J31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K31" t="s" s="0">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="L31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="M31" t="s" s="0">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="N31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O31" t="s" s="0">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="P31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Q31" t="s" s="0">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="R31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S31" t="s" s="0">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="T31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U31" t="s" s="0">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="V31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y31" t="s" s="0">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="Z31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AA31" t="s" s="0">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="AB31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC31" t="s" s="0">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="AD31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AE31" t="s" s="0">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="AF31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG31" t="s" s="0">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="AH31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI31" t="s" s="0">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="AJ31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AK31" t="s" s="0">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="AL31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM31" t="s" s="0">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="AN31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AO31" t="s" s="0">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="AP31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ31" t="s" s="0">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="AR31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS31" t="s" s="0">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="AT31" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW31" t="s" s="0">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="AX31" t="s" s="0">
         <v>51</v>
@@ -7258,94 +7336,131 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="J32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="K32" t="s" s="0">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="L32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="O32" t="s" s="0">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="P32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="S32" t="s" s="0">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="T32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="U32" t="s" s="0">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="V32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="Y32" t="s" s="0">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="Z32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AC32" t="s" s="0">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="AD32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AG32" t="s" s="0">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="AH32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AI32" t="s" s="0">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="AJ32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AM32" t="s" s="0">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="AN32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AQ32" t="s" s="0">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="AR32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AS32" t="s" s="0">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="AT32" t="s" s="0">
         <v>51</v>
       </c>
       <c r="AW32" t="s" s="0">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="AX32" t="s" s="0">
-        <v>51</v>
+        <v>554</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="AW35" t="s" s="0">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="AW36" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="AX36" t="n" s="0">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="AW37" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="AX37" t="n" s="0">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="AW38" t="s" s="0">
+        <v>554</v>
+      </c>
+      <c r="AX38" t="n" s="0">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="AW39" t="s" s="0">
+        <v>478</v>
+      </c>
+      <c r="AX39" t="n" s="0">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>